<commit_message>
add Export to Excel
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -6,18 +6,48 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Person" r:id="rId3" sheetId="1"/>
+    <sheet name="Client" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Name</t>
+    <t>id</t>
   </si>
   <si>
-    <t>Age</t>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>patronymic</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>registrationDate</t>
+  </si>
+  <si>
+    <t>lastVisitDate</t>
+  </si>
+  <si>
+    <t>countVisit</t>
+  </si>
+  <si>
+    <t>tags</t>
   </si>
   <si>
     <t>John Smith</t>
@@ -38,16 +68,25 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="16.0"/>
-      <b val="true"/>
+      <sz val="14.0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,22 +103,18 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="39.0625" customWidth="true"/>
-    <col min="2" max="2" width="19.53125" customWidth="true"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
@@ -88,10 +123,40 @@
       <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
+      <c r="C1" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B2" t="n">
         <v>20.0</v>

</xml_diff>